<commit_message>
fix parsing error with Aleph and Vav in source XML
</commit_message>
<xml_diff>
--- a/bible/nwt_xml/content.xlsx
+++ b/bible/nwt_xml/content.xlsx
@@ -515,11 +515,11 @@
   <dimension ref="A1:M68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N19" activeCellId="0" sqref="N19"/>
+      <selection pane="bottomLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
+      <selection pane="bottomRight" activeCell="J69" activeCellId="0" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -530,7 +530,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="7.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.83"/>
@@ -1350,11 +1351,21 @@
       <c r="E20" s="2" t="n">
         <v>150</v>
       </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="2"/>
+      <c r="F20" s="6" t="n">
+        <v>2461</v>
+      </c>
+      <c r="G20" s="6" t="n">
+        <v>3245</v>
+      </c>
+      <c r="H20" s="6" t="n">
+        <v>42286</v>
+      </c>
+      <c r="I20" s="6" t="n">
+        <v>176210</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>58</v>
+      </c>
       <c r="K20" s="2" t="n">
         <v>139.6</v>
       </c>
@@ -1363,7 +1374,7 @@
       </c>
       <c r="M20" s="7" t="n">
         <f aca="false">H20/L20</f>
-        <v>0</v>
+        <v>113.978436657682</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2609,23 +2620,23 @@
       </c>
       <c r="F68" s="6" t="n">
         <f aca="false">SUM(F2:F67)</f>
-        <v>15193</v>
+        <v>17654</v>
       </c>
       <c r="G68" s="6" t="n">
         <f aca="false">SUM(G2:G67)</f>
-        <v>20104</v>
+        <v>23349</v>
       </c>
       <c r="H68" s="6" t="n">
         <f aca="false">SUM(H2:H67)</f>
-        <v>393068</v>
+        <v>435354</v>
       </c>
       <c r="I68" s="6" t="n">
         <f aca="false">SUM(I2:I67)</f>
-        <v>1705534</v>
+        <v>1881744</v>
       </c>
       <c r="J68" s="6" t="n">
         <f aca="false">SUM(J2:J67)</f>
-        <v>551</v>
+        <v>609</v>
       </c>
       <c r="K68" s="6" t="n">
         <f aca="false">SUM(K2:K67)</f>
@@ -2637,7 +2648,7 @@
       </c>
       <c r="M68" s="7" t="n">
         <f aca="false">H68/L68</f>
-        <v>70.7848010084639</v>
+        <v>78.3997839005943</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated statistics for nwt
</commit_message>
<xml_diff>
--- a/bible/nwt_xml/content.xlsx
+++ b/bible/nwt_xml/content.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="nwt" sheetId="1" state="visible" r:id="rId3"/>
@@ -670,12 +670,12 @@
   </sheetPr>
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O16" activeCellId="0" sqref="O16"/>
+      <selection pane="bottomLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
+      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="B2:F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1976,7 +1976,7 @@
         <v>208</v>
       </c>
       <c r="H31" s="6" t="n">
-        <v>4288</v>
+        <v>4255</v>
       </c>
       <c r="I31" s="6" t="n">
         <v>18104</v>
@@ -1992,7 +1992,7 @@
       </c>
       <c r="M31" s="7" t="n">
         <f aca="false">H31/L31</f>
-        <v>142.933333333333</v>
+        <v>141.833333333333</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3275,7 +3275,7 @@
         <v>61</v>
       </c>
       <c r="G62" s="6" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="H62" s="6" t="n">
         <v>1681</v>
@@ -3528,11 +3528,11 @@
       </c>
       <c r="G68" s="6" t="n">
         <f aca="false">SUM(G2:G67)</f>
-        <v>42029</v>
+        <v>42032</v>
       </c>
       <c r="H68" s="6" t="n">
         <f aca="false">SUM(H2:H67)</f>
-        <v>789104</v>
+        <v>789071</v>
       </c>
       <c r="I68" s="6" t="n">
         <f aca="false">SUM(I2:I67)</f>
@@ -3552,7 +3552,7 @@
       </c>
       <c r="M68" s="7" t="n">
         <f aca="false">H68/L68</f>
-        <v>142.104087880425</v>
+        <v>142.098145146768</v>
       </c>
     </row>
   </sheetData>
@@ -3578,7 +3578,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
-      <selection pane="bottomRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B1" activeCellId="1" sqref="B2:F67 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5180,12 +5180,12 @@
   </sheetPr>
   <dimension ref="A1:U74"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2:F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7231,7 +7231,7 @@
         <v>208</v>
       </c>
       <c r="E31" s="15" t="n">
-        <v>4288</v>
+        <v>4255</v>
       </c>
       <c r="F31" s="15" t="n">
         <v>18104</v>
@@ -7273,7 +7273,7 @@
       </c>
       <c r="S31" s="15" t="n">
         <f aca="false">L31-E31</f>
-        <v>-68</v>
+        <v>-35</v>
       </c>
       <c r="T31" s="15" t="n">
         <f aca="false">M31-F31</f>
@@ -9305,7 +9305,7 @@
         <v>61</v>
       </c>
       <c r="D62" s="15" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E62" s="15" t="n">
         <v>1681</v>
@@ -9346,7 +9346,7 @@
       </c>
       <c r="R62" s="15" t="n">
         <f aca="false">K62-D62</f>
-        <v>-7</v>
+        <v>-10</v>
       </c>
       <c r="S62" s="15" t="n">
         <f aca="false">L62-E62</f>
@@ -9710,11 +9710,11 @@
       </c>
       <c r="D68" s="15" t="n">
         <f aca="false">SUM(D2:D67)</f>
-        <v>42029</v>
+        <v>42032</v>
       </c>
       <c r="E68" s="15" t="n">
         <f aca="false">SUM(E2:E67)</f>
-        <v>789104</v>
+        <v>789071</v>
       </c>
       <c r="F68" s="15" t="n">
         <f aca="false">SUM(F2:F67)</f>
@@ -9760,11 +9760,11 @@
       </c>
       <c r="R68" s="10" t="n">
         <f aca="false">SUM(R2:R67)</f>
-        <v>-6980</v>
+        <v>-6983</v>
       </c>
       <c r="S68" s="10" t="n">
         <f aca="false">SUM(S2:S67)</f>
-        <v>1469</v>
+        <v>1502</v>
       </c>
       <c r="T68" s="10" t="n">
         <f aca="false">SUM(T2:T67)</f>

</xml_diff>